<commit_message>
chiffre d'affaire et facturation
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/facturation.xlsx
+++ b/src/main/resources/templates/facturation.xlsx
@@ -610,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
@@ -722,9 +722,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
@@ -1050,7 +1047,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1078,7 +1075,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
@@ -1382,7 +1379,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G8" sqref="G8:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,7 +1407,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1436,9 +1433,9 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
-      <c r="J3" s="39"/>
-    </row>
-    <row r="4" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="J3" s="38"/>
+    </row>
+    <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
@@ -1482,7 +1479,7 @@
       </c>
       <c r="H5" s="21"/>
       <c r="I5" s="19"/>
-      <c r="J5" s="40" t="s">
+      <c r="J5" s="39" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1500,7 +1497,7 @@
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="27"/>
-      <c r="J6" s="41"/>
+      <c r="J6" s="40"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="29"/>
@@ -1524,7 +1521,7 @@
       <c r="I7" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="42"/>
+      <c r="J7" s="41"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
@@ -1542,9 +1539,13 @@
         <f>SUM(C8:E8)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="G8" s="33">
+        <v>0</v>
+      </c>
+      <c r="H8" s="33">
+        <v>0</v>
+      </c>
+      <c r="I8" s="33"/>
       <c r="J8" s="35">
         <f>SUM(G8:I8)</f>
         <v>0</v>
@@ -1566,9 +1567,9 @@
         <f t="shared" ref="F9:F16" si="0">SUM(C9:E9)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
       <c r="J9" s="35">
         <f t="shared" ref="J9:J16" si="1">SUM(G9:I9)</f>
         <v>0</v>
@@ -1590,9 +1591,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
       <c r="J10" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1614,9 +1615,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1638,9 +1639,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
       <c r="J12" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1658,9 +1659,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
       <c r="J13" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1678,9 +1679,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
       <c r="J14" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1700,9 +1701,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
       <c r="J15" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1720,9 +1721,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="35">
         <f t="shared" si="1"/>
         <v>0</v>

</xml_diff>